<commit_message>
Update on the code to be more clear....
</commit_message>
<xml_diff>
--- a/Mesures.xlsx
+++ b/Mesures.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\GitHub\IMTA-CD-Video_Compression_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F58CAAF-8624-440C-9B9D-4220E8D5E3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40049703-E12E-4054-BF3D-91E340823362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance compression image" sheetId="2" r:id="rId1"/>
+    <sheet name="Performance Motion vs Non Motio" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre de Frames</t>
   </si>
@@ -51,6 +52,15 @@
   </si>
   <si>
     <t>hours</t>
+  </si>
+  <si>
+    <t>Temps écoulé (s)</t>
+  </si>
+  <si>
+    <t>Qualité (%)</t>
+  </si>
+  <si>
+    <t>PSNR</t>
   </si>
 </sst>
 </file>
@@ -89,10 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,9 +144,966 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Performance compression image'!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance compression image'!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.1661319999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.419835</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5631010000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7186490000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9260710000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0306229999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2227480000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6204900000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.203767</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE76-4B1B-BAD1-2D873C846340}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="196402064"/>
+        <c:axId val="190957552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="196402064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Qualité de l'image Q (en %)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="190957552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="190957552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> écoulé (en sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="196402064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Performance!$A$2</c:f>
+              <c:f>'Performance compression image'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PSNR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Performance compression image'!$B$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance compression image'!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>26.3904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.917100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.574200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.760999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.746600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.757599999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.122100000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.203800000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41.235300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8E2-43BE-A62C-A832B7238580}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="127615536"/>
+        <c:axId val="1797953488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="127615536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Qualité de l'image Q (en %)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1797953488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1797953488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45"/>
+          <c:min val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>PSNR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="127615536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Motion vs Non Motio'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -158,7 +1126,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Performance!$B$1:$S$1</c:f>
+              <c:f>'Performance Motion vs Non Motio'!$B$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -221,7 +1189,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$B$2:$S$2</c:f>
+              <c:f>'Performance Motion vs Non Motio'!$B$2:$S$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -294,7 +1262,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Performance!$A$3</c:f>
+              <c:f>'Performance Motion vs Non Motio'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -320,7 +1288,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Performance!$B$1:$S$1</c:f>
+              <c:f>'Performance Motion vs Non Motio'!$B$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -383,7 +1351,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Performance!$B$3:$S$3</c:f>
+              <c:f>'Performance Motion vs Non Motio'!$B$3:$S$3</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="18"/>
@@ -808,6 +1776,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1324,7 +2372,1118 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{780AE668-A39F-4C14-8FB6-E18D1A51CE71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0131985-68C4-4840-873D-85B27AF25DED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1627,10 +3786,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FB7A3A-6D1B-451F-A27B-B64853245357}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>20</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>40</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+      <c r="G1">
+        <v>60</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+      <c r="I1">
+        <v>80</v>
+      </c>
+      <c r="J1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.1661319999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.419835</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.5631010000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.7186490000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.9260710000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.0306229999999998</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2.2227480000000002</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2.6204900000000002</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3.203767</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>26.3904</v>
+      </c>
+      <c r="C3" s="3">
+        <v>28.917100000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30.574200000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <v>31.760999999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>32.746600000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>33.757599999999996</v>
+      </c>
+      <c r="H3" s="3">
+        <v>35.122100000000003</v>
+      </c>
+      <c r="I3" s="3">
+        <v>37.203800000000001</v>
+      </c>
+      <c r="J3" s="3">
+        <v>41.235300000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to be more clear
</commit_message>
<xml_diff>
--- a/Mesures.xlsx
+++ b/Mesures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\GitHub\IMTA-CD-Video_Compression_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40049703-E12E-4054-BF3D-91E340823362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF0ACB6-5C33-4139-8B94-905371A72503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,7 +230,7 @@
           </c:trendline>
           <c:trendline>
             <c:spPr>
-              <a:ln w="22225" cap="rnd">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
@@ -714,6 +714,34 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'Performance compression image'!$B$1:$J$1</c:f>
@@ -3789,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FB7A3A-6D1B-451F-A27B-B64853245357}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>